<commit_message>
high voltage and current tests added
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="191029" fullCalcOnLoad="1"/>
+  <calcPr calcId="191028" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -51,7 +51,63 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="10">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -406,13 +462,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F109"/>
+  <dimension ref="A1:F163"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F73" sqref="F73"/>
+    <sheetView tabSelected="1" topLeftCell="A105" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B122" sqref="B122:D127"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.45"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -2510,13 +2566,1077 @@
         <v/>
       </c>
     </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>VH1</t>
+        </is>
+      </c>
+      <c r="B110" t="n">
+        <v>50</v>
+      </c>
+      <c r="C110" t="n">
+        <v>49.85</v>
+      </c>
+      <c r="D110" t="n">
+        <v>50.15</v>
+      </c>
+      <c r="E110" t="n">
+        <v>50</v>
+      </c>
+      <c r="F110">
+        <f>IF(AND(E110&gt;=C110,E110&lt;=D110), "PASS", "FAIL")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="111">
+      <c r="B111" t="n">
+        <v>100</v>
+      </c>
+      <c r="C111" t="n">
+        <v>99.7</v>
+      </c>
+      <c r="D111" t="n">
+        <v>100.3</v>
+      </c>
+      <c r="E111" t="n">
+        <v>100</v>
+      </c>
+      <c r="F111">
+        <f>IF(AND(E111&gt;=C111,E111&lt;=D111), "PASS", "FAIL")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="112">
+      <c r="B112" t="n">
+        <v>150</v>
+      </c>
+      <c r="C112" t="n">
+        <v>149.55</v>
+      </c>
+      <c r="D112" t="n">
+        <v>150.45</v>
+      </c>
+      <c r="E112" t="n">
+        <v>150</v>
+      </c>
+      <c r="F112">
+        <f>IF(AND(E112&gt;=C112,E112&lt;=D112), "PASS", "FAIL")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="113">
+      <c r="B113" t="n">
+        <v>200</v>
+      </c>
+      <c r="C113" t="n">
+        <v>199.4</v>
+      </c>
+      <c r="D113" t="n">
+        <v>200.6</v>
+      </c>
+      <c r="E113" t="n">
+        <v>200</v>
+      </c>
+      <c r="F113">
+        <f>IF(AND(E113&gt;=C113,E113&lt;=D113), "PASS", "FAIL")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="114">
+      <c r="B114" t="n">
+        <v>250</v>
+      </c>
+      <c r="C114" t="n">
+        <v>249.25</v>
+      </c>
+      <c r="D114" t="n">
+        <v>250.75</v>
+      </c>
+      <c r="E114" t="n">
+        <v>250</v>
+      </c>
+      <c r="F114">
+        <f>IF(AND(E114&gt;=C114,E114&lt;=D114), "PASS", "FAIL")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="115">
+      <c r="B115" t="n">
+        <v>300</v>
+      </c>
+      <c r="C115" t="n">
+        <v>299</v>
+      </c>
+      <c r="D115" t="n">
+        <v>301</v>
+      </c>
+      <c r="E115" t="n">
+        <v>301</v>
+      </c>
+      <c r="F115">
+        <f>IF(AND(E115&gt;=C115,E115&lt;=D115), "PASS", "FAIL")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>VH2</t>
+        </is>
+      </c>
+      <c r="B116" t="n">
+        <v>50</v>
+      </c>
+      <c r="C116" t="n">
+        <v>49.85</v>
+      </c>
+      <c r="D116" t="n">
+        <v>50.15</v>
+      </c>
+      <c r="E116" t="n">
+        <v>50</v>
+      </c>
+      <c r="F116">
+        <f>IF(AND(E116&gt;=C116,E116&lt;=D116), "PASS", "FAIL")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="117">
+      <c r="B117" t="n">
+        <v>100</v>
+      </c>
+      <c r="C117" t="n">
+        <v>99.7</v>
+      </c>
+      <c r="D117" t="n">
+        <v>100.3</v>
+      </c>
+      <c r="E117" t="n">
+        <v>100</v>
+      </c>
+      <c r="F117">
+        <f>IF(AND(E117&gt;=C117,E117&lt;=D117), "PASS", "FAIL")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="118">
+      <c r="B118" t="n">
+        <v>150</v>
+      </c>
+      <c r="C118" t="n">
+        <v>149.55</v>
+      </c>
+      <c r="D118" t="n">
+        <v>150.45</v>
+      </c>
+      <c r="E118" t="n">
+        <v>150</v>
+      </c>
+      <c r="F118">
+        <f>IF(AND(E118&gt;=C118,E118&lt;=D118), "PASS", "FAIL")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="119">
+      <c r="B119" t="n">
+        <v>200</v>
+      </c>
+      <c r="C119" t="n">
+        <v>199.4</v>
+      </c>
+      <c r="D119" t="n">
+        <v>200.6</v>
+      </c>
+      <c r="E119" t="n">
+        <v>200</v>
+      </c>
+      <c r="F119">
+        <f>IF(AND(E119&gt;=C119,E119&lt;=D119), "PASS", "FAIL")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="120">
+      <c r="B120" t="n">
+        <v>250</v>
+      </c>
+      <c r="C120" t="n">
+        <v>249.25</v>
+      </c>
+      <c r="D120" t="n">
+        <v>250.75</v>
+      </c>
+      <c r="E120" t="n">
+        <v>250</v>
+      </c>
+      <c r="F120">
+        <f>IF(AND(E120&gt;=C120,E120&lt;=D120), "PASS", "FAIL")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="121">
+      <c r="B121" t="n">
+        <v>300</v>
+      </c>
+      <c r="C121" t="n">
+        <v>299</v>
+      </c>
+      <c r="D121" t="n">
+        <v>301</v>
+      </c>
+      <c r="E121" t="n">
+        <v>301</v>
+      </c>
+      <c r="F121">
+        <f>IF(AND(E121&gt;=C121,E121&lt;=D121), "PASS", "FAIL")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>VH3</t>
+        </is>
+      </c>
+      <c r="B122" t="n">
+        <v>50</v>
+      </c>
+      <c r="C122" t="n">
+        <v>49.85</v>
+      </c>
+      <c r="D122" t="n">
+        <v>50.15</v>
+      </c>
+      <c r="E122" t="n">
+        <v>50</v>
+      </c>
+      <c r="F122">
+        <f>IF(AND(E122&gt;=C122,E122&lt;=D122), "PASS", "FAIL")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="123">
+      <c r="B123" t="n">
+        <v>100</v>
+      </c>
+      <c r="C123" t="n">
+        <v>99.7</v>
+      </c>
+      <c r="D123" t="n">
+        <v>100.3</v>
+      </c>
+      <c r="E123" t="n">
+        <v>100</v>
+      </c>
+      <c r="F123">
+        <f>IF(AND(E123&gt;=C123,E123&lt;=D123), "PASS", "FAIL")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="124">
+      <c r="B124" t="n">
+        <v>150</v>
+      </c>
+      <c r="C124" t="n">
+        <v>149.55</v>
+      </c>
+      <c r="D124" t="n">
+        <v>150.45</v>
+      </c>
+      <c r="E124" t="n">
+        <v>150</v>
+      </c>
+      <c r="F124">
+        <f>IF(AND(E124&gt;=C124,E124&lt;=D124), "PASS", "FAIL")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="125">
+      <c r="B125" t="n">
+        <v>200</v>
+      </c>
+      <c r="C125" t="n">
+        <v>199.4</v>
+      </c>
+      <c r="D125" t="n">
+        <v>200.6</v>
+      </c>
+      <c r="E125" t="n">
+        <v>200</v>
+      </c>
+      <c r="F125">
+        <f>IF(AND(E125&gt;=C125,E125&lt;=D125), "PASS", "FAIL")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="126">
+      <c r="B126" t="n">
+        <v>250</v>
+      </c>
+      <c r="C126" t="n">
+        <v>249.25</v>
+      </c>
+      <c r="D126" t="n">
+        <v>250.75</v>
+      </c>
+      <c r="E126" t="n">
+        <v>250</v>
+      </c>
+      <c r="F126">
+        <f>IF(AND(E126&gt;=C126,E126&lt;=D126), "PASS", "FAIL")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="127">
+      <c r="B127" t="n">
+        <v>300</v>
+      </c>
+      <c r="C127" t="n">
+        <v>299</v>
+      </c>
+      <c r="D127" t="n">
+        <v>301</v>
+      </c>
+      <c r="E127" t="n">
+        <v>301</v>
+      </c>
+      <c r="F127">
+        <f>IF(AND(E127&gt;=C127,E127&lt;=D127), "PASS", "FAIL")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>IH1</t>
+        </is>
+      </c>
+      <c r="B128" t="n">
+        <v>1</v>
+      </c>
+      <c r="C128" t="n">
+        <v>0.997</v>
+      </c>
+      <c r="D128" t="n">
+        <v>1.003</v>
+      </c>
+      <c r="E128" t="n">
+        <v>0.99952531</v>
+      </c>
+      <c r="F128">
+        <f>IF(AND(E128&gt;=C128,E128&lt;=D128), "PASS", "FAIL")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="129">
+      <c r="B129" t="n">
+        <v>2</v>
+      </c>
+      <c r="C129" t="n">
+        <v>1.994</v>
+      </c>
+      <c r="D129" t="n">
+        <v>2.006</v>
+      </c>
+      <c r="E129" t="n">
+        <v>1.99924719</v>
+      </c>
+      <c r="F129">
+        <f>IF(AND(E129&gt;=C129,E129&lt;=D129), "PASS", "FAIL")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="130">
+      <c r="B130" t="n">
+        <v>3</v>
+      </c>
+      <c r="C130" t="n">
+        <v>2.991</v>
+      </c>
+      <c r="D130" t="n">
+        <v>3.009</v>
+      </c>
+      <c r="E130" t="n">
+        <v>2.9996326</v>
+      </c>
+      <c r="F130">
+        <f>IF(AND(E130&gt;=C130,E130&lt;=D130), "PASS", "FAIL")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="131">
+      <c r="B131" t="n">
+        <v>4</v>
+      </c>
+      <c r="C131" t="n">
+        <v>3.988</v>
+      </c>
+      <c r="D131" t="n">
+        <v>4.012</v>
+      </c>
+      <c r="E131" t="n">
+        <v>3.99974108</v>
+      </c>
+      <c r="F131">
+        <f>IF(AND(E131&gt;=C131,E131&lt;=D131), "PASS", "FAIL")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="132">
+      <c r="B132" t="n">
+        <v>5</v>
+      </c>
+      <c r="C132" t="n">
+        <v>4.985</v>
+      </c>
+      <c r="D132" t="n">
+        <v>5.015</v>
+      </c>
+      <c r="E132" t="n">
+        <v>5.00013781</v>
+      </c>
+      <c r="F132">
+        <f>IF(AND(E132&gt;=C132,E132&lt;=D132), "PASS", "FAIL")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="133">
+      <c r="B133" t="n">
+        <v>6</v>
+      </c>
+      <c r="C133" t="n">
+        <v>5.982</v>
+      </c>
+      <c r="D133" t="n">
+        <v>6.018</v>
+      </c>
+      <c r="E133" t="n">
+        <v>6.00014973</v>
+      </c>
+      <c r="F133">
+        <f>IF(AND(E133&gt;=C133,E133&lt;=D133), "PASS", "FAIL")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>IH2</t>
+        </is>
+      </c>
+      <c r="B134" t="n">
+        <v>1</v>
+      </c>
+      <c r="C134" t="n">
+        <v>0.997</v>
+      </c>
+      <c r="D134" t="n">
+        <v>1.003</v>
+      </c>
+      <c r="E134" t="n">
+        <v>0.9997226</v>
+      </c>
+      <c r="F134">
+        <f>IF(AND(E134&gt;=C134,E134&lt;=D134), "PASS", "FAIL")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="135">
+      <c r="B135" t="n">
+        <v>2</v>
+      </c>
+      <c r="C135" t="n">
+        <v>1.994</v>
+      </c>
+      <c r="D135" t="n">
+        <v>2.006</v>
+      </c>
+      <c r="E135" t="n">
+        <v>1.9996196</v>
+      </c>
+      <c r="F135">
+        <f>IF(AND(E135&gt;=C135,E135&lt;=D135), "PASS", "FAIL")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="136">
+      <c r="B136" t="n">
+        <v>3</v>
+      </c>
+      <c r="C136" t="n">
+        <v>2.991</v>
+      </c>
+      <c r="D136" t="n">
+        <v>3.009</v>
+      </c>
+      <c r="E136" t="n">
+        <v>3.00004983</v>
+      </c>
+      <c r="F136">
+        <f>IF(AND(E136&gt;=C136,E136&lt;=D136), "PASS", "FAIL")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="137">
+      <c r="B137" t="n">
+        <v>4</v>
+      </c>
+      <c r="C137" t="n">
+        <v>3.988</v>
+      </c>
+      <c r="D137" t="n">
+        <v>4.012</v>
+      </c>
+      <c r="E137" t="n">
+        <v>4.0004735</v>
+      </c>
+      <c r="F137">
+        <f>IF(AND(E137&gt;=C137,E137&lt;=D137), "PASS", "FAIL")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="138">
+      <c r="B138" t="n">
+        <v>5</v>
+      </c>
+      <c r="C138" t="n">
+        <v>4.985</v>
+      </c>
+      <c r="D138" t="n">
+        <v>5.015</v>
+      </c>
+      <c r="E138" t="n">
+        <v>5.00082779</v>
+      </c>
+      <c r="F138">
+        <f>IF(AND(E138&gt;=C138,E138&lt;=D138), "PASS", "FAIL")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="139">
+      <c r="B139" t="n">
+        <v>6</v>
+      </c>
+      <c r="C139" t="n">
+        <v>5.982</v>
+      </c>
+      <c r="D139" t="n">
+        <v>6.018</v>
+      </c>
+      <c r="E139" t="n">
+        <v>6.00077391</v>
+      </c>
+      <c r="F139">
+        <f>IF(AND(E139&gt;=C139,E139&lt;=D139), "PASS", "FAIL")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>IH3</t>
+        </is>
+      </c>
+      <c r="B140" t="n">
+        <v>1</v>
+      </c>
+      <c r="C140" t="n">
+        <v>0.997</v>
+      </c>
+      <c r="D140" t="n">
+        <v>1.003</v>
+      </c>
+      <c r="E140" t="n">
+        <v>0.99990565</v>
+      </c>
+      <c r="F140">
+        <f>IF(AND(E140&gt;=C140,E140&lt;=D140), "PASS", "FAIL")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="141">
+      <c r="B141" t="n">
+        <v>2</v>
+      </c>
+      <c r="C141" t="n">
+        <v>1.994</v>
+      </c>
+      <c r="D141" t="n">
+        <v>2.006</v>
+      </c>
+      <c r="E141" t="n">
+        <v>1.99978471</v>
+      </c>
+      <c r="F141">
+        <f>IF(AND(E141&gt;=C141,E141&lt;=D141), "PASS", "FAIL")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="142">
+      <c r="B142" t="n">
+        <v>3</v>
+      </c>
+      <c r="C142" t="n">
+        <v>2.991</v>
+      </c>
+      <c r="D142" t="n">
+        <v>3.009</v>
+      </c>
+      <c r="E142" t="n">
+        <v>3.00055504</v>
+      </c>
+      <c r="F142">
+        <f>IF(AND(E142&gt;=C142,E142&lt;=D142), "PASS", "FAIL")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="143">
+      <c r="B143" t="n">
+        <v>4</v>
+      </c>
+      <c r="C143" t="n">
+        <v>3.988</v>
+      </c>
+      <c r="D143" t="n">
+        <v>4.012</v>
+      </c>
+      <c r="E143" t="n">
+        <v>4.00096369</v>
+      </c>
+      <c r="F143">
+        <f>IF(AND(E143&gt;=C143,E143&lt;=D143), "PASS", "FAIL")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="144">
+      <c r="B144" t="n">
+        <v>5</v>
+      </c>
+      <c r="C144" t="n">
+        <v>4.985</v>
+      </c>
+      <c r="D144" t="n">
+        <v>5.015</v>
+      </c>
+      <c r="E144" t="n">
+        <v>5.00128889</v>
+      </c>
+      <c r="F144">
+        <f>IF(AND(E144&gt;=C144,E144&lt;=D144), "PASS", "FAIL")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="145">
+      <c r="B145" t="n">
+        <v>6</v>
+      </c>
+      <c r="C145" t="n">
+        <v>5.982</v>
+      </c>
+      <c r="D145" t="n">
+        <v>6.018</v>
+      </c>
+      <c r="E145" t="n">
+        <v>6.00170803</v>
+      </c>
+      <c r="F145">
+        <f>IF(AND(E145&gt;=C145,E145&lt;=D145), "PASS", "FAIL")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>Phase(VH1)</t>
+        </is>
+      </c>
+      <c r="B146" t="n">
+        <v>60</v>
+      </c>
+      <c r="C146" t="n">
+        <v>59.75</v>
+      </c>
+      <c r="D146" t="n">
+        <v>60.25</v>
+      </c>
+      <c r="E146" t="n">
+        <v>60.26304637721221</v>
+      </c>
+      <c r="F146">
+        <f>IF(AND(E146&gt;=C146,E146&lt;=D146), "PASS", "FAIL")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="147">
+      <c r="B147" t="n">
+        <v>120</v>
+      </c>
+      <c r="C147" t="n">
+        <v>119.75</v>
+      </c>
+      <c r="D147" t="n">
+        <v>120.25</v>
+      </c>
+      <c r="E147" t="n">
+        <v>120.2972119614733</v>
+      </c>
+      <c r="F147">
+        <f>IF(AND(E147&gt;=C147,E147&lt;=D147), "PASS", "FAIL")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="148">
+      <c r="B148" t="n">
+        <v>180</v>
+      </c>
+      <c r="C148" t="n">
+        <v>179.75</v>
+      </c>
+      <c r="D148" t="n">
+        <v>180.25</v>
+      </c>
+      <c r="E148" t="n">
+        <v>179.7593575491723</v>
+      </c>
+      <c r="F148">
+        <f>IF(AND(E148&gt;=C148,E148&lt;=D148), "PASS", "FAIL")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>Phase(VH2)</t>
+        </is>
+      </c>
+      <c r="B149" t="n">
+        <v>60</v>
+      </c>
+      <c r="C149" t="n">
+        <v>59.75</v>
+      </c>
+      <c r="D149" t="n">
+        <v>60.25</v>
+      </c>
+      <c r="E149" t="n">
+        <v>60.23295852263566</v>
+      </c>
+      <c r="F149">
+        <f>IF(AND(E149&gt;=C149,E149&lt;=D149), "PASS", "FAIL")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="150">
+      <c r="B150" t="n">
+        <v>120</v>
+      </c>
+      <c r="C150" t="n">
+        <v>119.75</v>
+      </c>
+      <c r="D150" t="n">
+        <v>120.25</v>
+      </c>
+      <c r="E150" t="n">
+        <v>120.2331134184667</v>
+      </c>
+      <c r="F150">
+        <f>IF(AND(E150&gt;=C150,E150&lt;=D150), "PASS", "FAIL")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="151">
+      <c r="B151" t="n">
+        <v>180</v>
+      </c>
+      <c r="C151" t="n">
+        <v>179.75</v>
+      </c>
+      <c r="D151" t="n">
+        <v>180.25</v>
+      </c>
+      <c r="E151" t="n">
+        <v>179.768394454297</v>
+      </c>
+      <c r="F151">
+        <f>IF(AND(E151&gt;=C151,E151&lt;=D151), "PASS", "FAIL")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>Phase(VH3)</t>
+        </is>
+      </c>
+      <c r="B152" t="n">
+        <v>60</v>
+      </c>
+      <c r="C152" t="n">
+        <v>59.75</v>
+      </c>
+      <c r="D152" t="n">
+        <v>60.25</v>
+      </c>
+      <c r="E152" t="n">
+        <v>60.21943581112865</v>
+      </c>
+      <c r="F152">
+        <f>IF(AND(E152&gt;=C152,E152&lt;=D152), "PASS", "FAIL")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="153">
+      <c r="B153" t="n">
+        <v>120</v>
+      </c>
+      <c r="C153" t="n">
+        <v>119.75</v>
+      </c>
+      <c r="D153" t="n">
+        <v>120.25</v>
+      </c>
+      <c r="E153" t="n">
+        <v>120.2084549933066</v>
+      </c>
+      <c r="F153">
+        <f>IF(AND(E153&gt;=C153,E153&lt;=D153), "PASS", "FAIL")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="154">
+      <c r="B154" t="n">
+        <v>180</v>
+      </c>
+      <c r="C154" t="n">
+        <v>179.75</v>
+      </c>
+      <c r="D154" t="n">
+        <v>180.25</v>
+      </c>
+      <c r="E154" t="n">
+        <v>179.8082515568856</v>
+      </c>
+      <c r="F154">
+        <f>IF(AND(E154&gt;=C154,E154&lt;=D154), "PASS", "FAIL")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>Phase(IH1)</t>
+        </is>
+      </c>
+      <c r="B155" t="n">
+        <v>60</v>
+      </c>
+      <c r="C155" t="n">
+        <v>59.75</v>
+      </c>
+      <c r="D155" t="n">
+        <v>60.25</v>
+      </c>
+      <c r="E155" t="n">
+        <v>60.2292403880278</v>
+      </c>
+      <c r="F155">
+        <f>IF(AND(E155&gt;=C155,E155&lt;=D155), "PASS", "FAIL")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="156">
+      <c r="B156" t="n">
+        <v>120</v>
+      </c>
+      <c r="C156" t="n">
+        <v>119.75</v>
+      </c>
+      <c r="D156" t="n">
+        <v>120.25</v>
+      </c>
+      <c r="E156" t="n">
+        <v>120.2336267040371</v>
+      </c>
+      <c r="F156">
+        <f>IF(AND(E156&gt;=C156,E156&lt;=D156), "PASS", "FAIL")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="157">
+      <c r="B157" t="n">
+        <v>180</v>
+      </c>
+      <c r="C157" t="n">
+        <v>179.75</v>
+      </c>
+      <c r="D157" t="n">
+        <v>180.25</v>
+      </c>
+      <c r="E157" t="n">
+        <v>179.7770611051297</v>
+      </c>
+      <c r="F157">
+        <f>IF(AND(E157&gt;=C157,E157&lt;=D157), "PASS", "FAIL")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>Phase(IH2)</t>
+        </is>
+      </c>
+      <c r="B158" t="n">
+        <v>60</v>
+      </c>
+      <c r="C158" t="n">
+        <v>59.75</v>
+      </c>
+      <c r="D158" t="n">
+        <v>60.25</v>
+      </c>
+      <c r="E158" t="n">
+        <v>59.80549734096019</v>
+      </c>
+      <c r="F158">
+        <f>IF(AND(E158&gt;=C158,E158&lt;=D158), "PASS", "FAIL")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="159">
+      <c r="B159" t="n">
+        <v>120</v>
+      </c>
+      <c r="C159" t="n">
+        <v>119.75</v>
+      </c>
+      <c r="D159" t="n">
+        <v>120.25</v>
+      </c>
+      <c r="E159" t="n">
+        <v>119.7908741234901</v>
+      </c>
+      <c r="F159">
+        <f>IF(AND(E159&gt;=C159,E159&lt;=D159), "PASS", "FAIL")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="160">
+      <c r="B160" t="n">
+        <v>180</v>
+      </c>
+      <c r="C160" t="n">
+        <v>179.75</v>
+      </c>
+      <c r="D160" t="n">
+        <v>180.25</v>
+      </c>
+      <c r="E160" t="n">
+        <v>179.8241476184619</v>
+      </c>
+      <c r="F160">
+        <f>IF(AND(E160&gt;=C160,E160&lt;=D160), "PASS", "FAIL")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>Phase(IH3)</t>
+        </is>
+      </c>
+      <c r="B161" t="n">
+        <v>60</v>
+      </c>
+      <c r="C161" t="n">
+        <v>59.75</v>
+      </c>
+      <c r="D161" t="n">
+        <v>60.25</v>
+      </c>
+      <c r="E161" t="n">
+        <v>59.78603605450781</v>
+      </c>
+      <c r="F161">
+        <f>IF(AND(E161&gt;=C161,E161&lt;=D161), "PASS", "FAIL")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="162">
+      <c r="B162" t="n">
+        <v>120</v>
+      </c>
+      <c r="C162" t="n">
+        <v>119.75</v>
+      </c>
+      <c r="D162" t="n">
+        <v>120.25</v>
+      </c>
+      <c r="E162" t="n">
+        <v>119.7979768913345</v>
+      </c>
+      <c r="F162">
+        <f>IF(AND(E162&gt;=C162,E162&lt;=D162), "PASS", "FAIL")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="163">
+      <c r="B163" t="n">
+        <v>180</v>
+      </c>
+      <c r="C163" t="n">
+        <v>179.75</v>
+      </c>
+      <c r="D163" t="n">
+        <v>180.25</v>
+      </c>
+      <c r="E163" t="n">
+        <v>179.8031824372122</v>
+      </c>
+      <c r="F163">
+        <f>IF(AND(E163&gt;=C163,E163&lt;=D163), "PASS", "FAIL")</f>
+        <v/>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="F2:F109">
-    <cfRule type="containsText" priority="23" operator="containsText" dxfId="1" text="FAIL">
+  <conditionalFormatting sqref="F2:F118">
+    <cfRule type="containsText" priority="31" operator="containsText" dxfId="1" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",F2)))</formula>
     </cfRule>
-    <cfRule type="containsText" priority="24" operator="containsText" dxfId="0" text="PASS">
+    <cfRule type="containsText" priority="32" operator="containsText" dxfId="0" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",F2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F119:F127">
+    <cfRule type="containsText" priority="7" operator="containsText" dxfId="1" text="FAIL">
+      <formula>NOT(ISERROR(SEARCH("FAIL",F119)))</formula>
+    </cfRule>
+    <cfRule type="containsText" priority="8" operator="containsText" dxfId="0" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",F119)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F128:F145">
+    <cfRule type="containsText" priority="5" operator="containsText" dxfId="1" text="FAIL">
+      <formula>NOT(ISERROR(SEARCH("FAIL",F128)))</formula>
+    </cfRule>
+    <cfRule type="containsText" priority="6" operator="containsText" dxfId="0" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",F128)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F146:F154">
+    <cfRule type="containsText" priority="3" operator="containsText" dxfId="1" text="FAIL">
+      <formula>NOT(ISERROR(SEARCH("FAIL",F146)))</formula>
+    </cfRule>
+    <cfRule type="containsText" priority="4" operator="containsText" dxfId="0" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",F146)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F155:F163">
+    <cfRule type="containsText" priority="1" operator="containsText" dxfId="1" text="FAIL">
+      <formula>NOT(ISERROR(SEARCH("FAIL",F155)))</formula>
+    </cfRule>
+    <cfRule type="containsText" priority="2" operator="containsText" dxfId="0" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",F155)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>